<commit_message>
fixed strange issues with generation added drawing with decal, needs to be finished
</commit_message>
<xml_diff>
--- a/Tile Drawing Calculatoer.xlsx
+++ b/Tile Drawing Calculatoer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Personal Projects\Shipping\shipping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFFE5F3-E5DF-4412-9512-7734ACBEFC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9CADAF-F48E-41BA-8A29-579B590329F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="8550" windowWidth="18000" windowHeight="9360" xr2:uid="{FA220E38-1FB6-4857-AE92-025EBD43C4A0}"/>
+    <workbookView xWindow="5130" yWindow="1065" windowWidth="18000" windowHeight="9360" xr2:uid="{FA220E38-1FB6-4857-AE92-025EBD43C4A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,19 +487,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>500</v>
+        <v>525</v>
       </c>
       <c r="C2" s="4">
-        <v>500</v>
+        <v>525</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="6">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="F2" s="6">
-        <v>-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -508,11 +508,11 @@
       </c>
       <c r="B3">
         <f>B2-250</f>
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="C3">
         <f>C2-250</f>
-        <v>250</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -521,11 +521,11 @@
       </c>
       <c r="B5">
         <f>CEILING(B2/50,1)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <f>CEILING(C2/50,1)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -534,11 +534,11 @@
       </c>
       <c r="B6">
         <f>B5+E2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <f>C5+F2</f>
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -547,11 +547,11 @@
       </c>
       <c r="B7">
         <f>B6*50</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C7">
         <f>C6*50</f>
-        <v>200</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -560,11 +560,11 @@
       </c>
       <c r="B9" s="2">
         <f>B7-B3</f>
-        <v>-50</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2">
         <f>C7-C3</f>
-        <v>-50</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>